<commit_message>
Antes de agregar electron
</commit_message>
<xml_diff>
--- a/BACKEND/uploads/archivo_subido.xlsx
+++ b/BACKEND/uploads/archivo_subido.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\registrolagranja\Documents\certificados-la-granja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\registrolagranja\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D806A1-F93D-4B72-9910-60BF3EC1F5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D34AF7-D73F-4247-949B-0942F0BE4377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
   <si>
     <t>TIPO DE DOCUMENTO</t>
   </si>
@@ -28,7 +28,7 @@
     <t>NUMERO DE DOCUMENTO</t>
   </si>
   <si>
-    <t>NOMBRES  Y APELLIDOS</t>
+    <t>NOMBRE  Y APELLIDO</t>
   </si>
   <si>
     <t>DIA</t>
@@ -89,6 +89,126 @@
   </si>
   <si>
     <t>ANA DE JESUS SUAREZ NUÑEZ</t>
+  </si>
+  <si>
+    <t>NIEVES OSORIO ANDRADE</t>
+  </si>
+  <si>
+    <t>NELSON COCOMA GUTIERREZ</t>
+  </si>
+  <si>
+    <t>ENERO</t>
+  </si>
+  <si>
+    <t>MARIA ROSELITA GARZON TORRES</t>
+  </si>
+  <si>
+    <t>MARTHA CECILIA OVIEDO CUMACO</t>
+  </si>
+  <si>
+    <t>FRANCISCO JAVIER BUITRAGO ALZATE</t>
+  </si>
+  <si>
+    <t>ANA LILIA MENDOZA PERALTA</t>
+  </si>
+  <si>
+    <t>OCTUBRE</t>
+  </si>
+  <si>
+    <t>FLOR ANGELA SUAREZ</t>
+  </si>
+  <si>
+    <t>JOSE CARLOS CUASPUD CUARAN</t>
+  </si>
+  <si>
+    <t>CARMEN CECILIA CUASPUD CUARAN</t>
+  </si>
+  <si>
+    <t>FEBRERO</t>
+  </si>
+  <si>
+    <t>JULIA ELVIRA DE LAS MERCEDES RIVERA DE BONILLA</t>
+  </si>
+  <si>
+    <t>ABRIL</t>
+  </si>
+  <si>
+    <t>MARIA DEL CARMEN CUMACO</t>
+  </si>
+  <si>
+    <t>MARZO</t>
+  </si>
+  <si>
+    <t>ROSALIA BONILLA BERNAL</t>
+  </si>
+  <si>
+    <t>JOSE ANGEL CORTES</t>
+  </si>
+  <si>
+    <t>MARIA GUIOMAR DELGADO</t>
+  </si>
+  <si>
+    <t>MARIA CECILIA LINARES DE RUIZ</t>
+  </si>
+  <si>
+    <t>BLANCA DORIS MARIN CARVAJAL</t>
+  </si>
+  <si>
+    <t>MARIA EMMA FERNANDEZ DE BERMUDEZ</t>
+  </si>
+  <si>
+    <t>LUCY CHAPARRO</t>
+  </si>
+  <si>
+    <t>AUGUSTO ACOSTA ROCHA</t>
+  </si>
+  <si>
+    <t>JUNIO</t>
+  </si>
+  <si>
+    <t>ARMANDO DAZA</t>
+  </si>
+  <si>
+    <t>MABEL CRUZ PULIDO</t>
+  </si>
+  <si>
+    <t>ELVIA GUALTEROS DE CARDENAS</t>
+  </si>
+  <si>
+    <t>MARIA ROSA QUIÑONES VARON</t>
+  </si>
+  <si>
+    <t>ANA BERTILDA CIFUENTES</t>
+  </si>
+  <si>
+    <t>LILIA CARDOSO</t>
+  </si>
+  <si>
+    <t>GLADYS MORA DE MOLINA</t>
+  </si>
+  <si>
+    <t>IRENE VALENCIA BEDOYA</t>
+  </si>
+  <si>
+    <t>ROSA MARIA MORENO</t>
+  </si>
+  <si>
+    <t>MARIA ANTONIA DIAZ DE MORENO</t>
+  </si>
+  <si>
+    <t>MIGUEL ANGEL SERRATO ORTIZ</t>
+  </si>
+  <si>
+    <t>ARANZAZU GUZMAN DE SERRATE</t>
+  </si>
+  <si>
+    <t>ALIRIO DUCUARA</t>
+  </si>
+  <si>
+    <t>JAVIER ALDANA VERA</t>
+  </si>
+  <si>
+    <t>GLADYS STELLA ACOSTA BARRIOS</t>
   </si>
 </sst>
 </file>
@@ -98,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +230,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -153,15 +279,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -465,17 +592,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
     <col min="4" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -504,7 +631,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>110845316</v>
+        <v>1108453116</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -699,7 +826,688 @@
         <v>1973</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3">
+        <v>28561477</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4">
+        <v>14214360</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4">
+        <v>28535943</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4">
+        <v>38259203</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4">
+        <v>3527624</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4">
+        <v>41309022</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="4">
+        <v>41385637</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4">
+        <v>5309168</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4">
+        <v>27086690</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4">
+        <v>28533186</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="4">
+        <v>38245927</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4">
+        <v>65711349</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="4">
+        <v>2399228</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="4">
+        <v>65776653</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="4">
+        <v>41679421</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="4">
+        <v>38218985</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="4">
+        <v>28534877</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="4">
+        <v>38229591</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="4">
+        <v>14202804</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="4">
+        <v>5836245</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="4">
+        <v>38251449</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32">
+        <v>22</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="4">
+        <v>24147995</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="4">
+        <v>38228377</v>
+      </c>
+      <c r="C34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34">
+        <v>24</v>
+      </c>
+      <c r="E34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="4">
+        <v>28529541</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="4">
+        <v>65736627</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="4">
+        <v>38253343</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37">
+        <v>27</v>
+      </c>
+      <c r="E37" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="4">
+        <v>28944793</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38">
+        <v>25</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="4">
+        <v>41487086</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39">
+        <v>18</v>
+      </c>
+      <c r="E39" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="4">
+        <v>20870721</v>
+      </c>
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="4">
+        <v>19235938</v>
+      </c>
+      <c r="C41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41">
+        <v>21</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="4">
+        <v>28682077</v>
+      </c>
+      <c r="C42" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42">
+        <v>20</v>
+      </c>
+      <c r="E42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="4">
+        <v>14228825</v>
+      </c>
+      <c r="C43" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="4">
+        <v>14256241</v>
+      </c>
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="4">
+        <v>38241672</v>
+      </c>
+      <c r="C45" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45">
+        <v>22</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45">
+        <v>1977</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ventana cuando acaba la automatizacion
</commit_message>
<xml_diff>
--- a/BACKEND/uploads/archivo_subido.xlsx
+++ b/BACKEND/uploads/archivo_subido.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\registrolagranja\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\registrolagranja\Documents\CertiGranja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E2F1F4-E200-4A38-BAC6-AE58679F3611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F52775-7DE6-47AA-BAB3-78A983701399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="4500" windowWidth="15690" windowHeight="10410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>TIPO DE DOCUMENTO</t>
   </si>
@@ -52,24 +52,6 @@
     <t>MARLON MOSQUERA</t>
   </si>
   <si>
-    <t xml:space="preserve">GERMAN LOPEZ </t>
-  </si>
-  <si>
-    <t>DICIEMBRE</t>
-  </si>
-  <si>
-    <t>CARMEN ROSA GARCIA BRAVO</t>
-  </si>
-  <si>
-    <t>AGOSTO</t>
-  </si>
-  <si>
-    <t>JAIME LOPEZ GOMEZ</t>
-  </si>
-  <si>
-    <t>JULIO</t>
-  </si>
-  <si>
     <t>SARA DIAZ RIVERA</t>
   </si>
   <si>
@@ -77,18 +59,6 @@
   </si>
   <si>
     <t>SEPTIEMBRE</t>
-  </si>
-  <si>
-    <t>AYDEE DE JESUS GIRALDO MENDEZ</t>
-  </si>
-  <si>
-    <t>CARMEN BASTO MORALES</t>
-  </si>
-  <si>
-    <t>NOVIEMBRE</t>
-  </si>
-  <si>
-    <t>ANA DE JESUS SUAREZ NUÑEZ</t>
   </si>
 </sst>
 </file>
@@ -155,12 +125,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -465,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,20 +511,20 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>5813300</v>
+      <c r="B4" s="2">
+        <v>38222588</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F4">
-        <v>1961</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -563,139 +532,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>38237961</v>
+        <v>41587804</v>
       </c>
       <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
       <c r="F5">
-        <v>1977</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <v>6000297</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6">
-        <v>1975</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <v>38222588</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>1973</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3">
-        <v>41587804</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8">
         <v>1974</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3">
-        <v>38215199</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9">
-        <v>1970</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3">
-        <v>65496347</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10">
-        <v>1978</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3">
-        <v>28953763</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11">
-        <v>1973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
es mas rapido gracias a MM
</commit_message>
<xml_diff>
--- a/BACKEND/uploads/archivo_subido.xlsx
+++ b/BACKEND/uploads/archivo_subido.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\registrolagranja\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64B48B4-0581-4D63-B418-871E21DD1AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501D726A-4B8D-4EC8-9397-EB7A8758D68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="23385" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>TIPO DE DOCUMENTO</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>MAYO</t>
+  </si>
+  <si>
+    <t>HP</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,6 +465,26 @@
         <v>2024</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1108453116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>2024</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Modulo de agregar ficha completado
</commit_message>
<xml_diff>
--- a/BACKEND/uploads/archivo_subido.xlsx
+++ b/BACKEND/uploads/archivo_subido.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="0" windowWidth="16875" windowHeight="8265"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="16875" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>TIPO DE DOCUMENTO</t>
   </si>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,6 +471,29 @@
         <v>2671143</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1070593778</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>2024</v>
+      </c>
+      <c r="G3">
+        <v>2671143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revivimos, crea carpeta y los resultados guardan en la carpeta
</commit_message>
<xml_diff>
--- a/BACKEND/uploads/archivo_subido.xlsx
+++ b/BACKEND/uploads/archivo_subido.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\registrolagranja\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sena\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C89057-AB12-4D27-BAC2-5BE7E1FF3CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52D7F48-6971-43DA-8261-DB7860374F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3240" windowWidth="23385" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>TIPO DE DOCUMENTO</t>
   </si>
@@ -40,16 +40,19 @@
     <t>AÑO</t>
   </si>
   <si>
-    <t>FICHA</t>
+    <t>ABRIL</t>
+  </si>
+  <si>
+    <t>ENERO</t>
+  </si>
+  <si>
+    <t>NOVIEMBRE</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t>CC</t>
-  </si>
-  <si>
-    <t>YISEL CARINA ALBA DIAZ</t>
-  </si>
-  <si>
-    <t>JULIO</t>
   </si>
 </sst>
 </file>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +429,7 @@
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,31 +448,105 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>28901342</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>20290328</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>1110545531</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
       </c>
+      <c r="F4">
+        <v>2012</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>24486494</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>1106773397</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F5">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>94516719</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2">
-        <v>2024</v>
-      </c>
-      <c r="G2">
-        <v>123</v>
+      <c r="F6">
+        <v>1996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PDFS EN LA CARPETA Y LOS UNE
</commit_message>
<xml_diff>
--- a/BACKEND/uploads/archivo_subido.xlsx
+++ b/BACKEND/uploads/archivo_subido.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sena\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52D7F48-6971-43DA-8261-DB7860374F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571D1645-DA05-4F96-9618-EB239E2EB116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +506,7 @@
         <v>6</v>
       </c>
       <c r="F4">
-        <v>2012</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tratando de resolver lo de la pagina caida
</commit_message>
<xml_diff>
--- a/BACKEND/uploads/archivo_subido.xlsx
+++ b/BACKEND/uploads/archivo_subido.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sena\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yair\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571D1645-DA05-4F96-9618-EB239E2EB116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F563E4F2-B236-4490-8AFF-BF3070900A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="16">
   <si>
     <t>TIPO DE DOCUMENTO</t>
   </si>
@@ -43,10 +43,25 @@
     <t>ABRIL</t>
   </si>
   <si>
+    <t>SEPTIEMBRE</t>
+  </si>
+  <si>
+    <t>JULIO</t>
+  </si>
+  <si>
+    <t>JUNIO</t>
+  </si>
+  <si>
+    <t>FEBRERO</t>
+  </si>
+  <si>
     <t>ENERO</t>
   </si>
   <si>
     <t>NOVIEMBRE</t>
+  </si>
+  <si>
+    <t>AGOSTO</t>
   </si>
   <si>
     <t>NA</t>
@@ -415,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +441,6 @@
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="3" width="29" customWidth="1"/>
     <col min="4" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -451,19 +465,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>28901342</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>1978</v>
@@ -471,19 +485,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>20290328</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F3">
         <v>1963</v>
@@ -491,13 +505,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>1110545531</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -511,19 +525,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>24486494</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <v>1976</v>
@@ -531,22 +545,322 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>94516719</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>1996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>38253096</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>65769149</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>1110574193</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1110549747</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1617567</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>65735017</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>12185483</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>41922408</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>28612802</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>28603778</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>65733352</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>28604216</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>38257409</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>65738644</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>38261159</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>1982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglos al unir certificados
</commit_message>
<xml_diff>
--- a/BACKEND/uploads/archivo_subido.xlsx
+++ b/BACKEND/uploads/archivo_subido.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yair\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sena\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F563E4F2-B236-4490-8AFF-BF3070900A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4966E4C-237C-439E-9900-127208774F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="18">
   <si>
     <t>TIPO DE DOCUMENTO</t>
   </si>
@@ -40,34 +40,40 @@
     <t>AÑO</t>
   </si>
   <si>
+    <t>FEBRERO</t>
+  </si>
+  <si>
     <t>ABRIL</t>
   </si>
   <si>
+    <t>NOVIEMBRE</t>
+  </si>
+  <si>
+    <t>JUNIO</t>
+  </si>
+  <si>
+    <t>AGOSTO</t>
+  </si>
+  <si>
+    <t>DICIEMBRE</t>
+  </si>
+  <si>
     <t>SEPTIEMBRE</t>
   </si>
   <si>
+    <t>MAYO</t>
+  </si>
+  <si>
+    <t>OCTUBRE</t>
+  </si>
+  <si>
     <t>JULIO</t>
   </si>
   <si>
-    <t>JUNIO</t>
-  </si>
-  <si>
-    <t>FEBRERO</t>
-  </si>
-  <si>
-    <t>ENERO</t>
-  </si>
-  <si>
-    <t>NOVIEMBRE</t>
-  </si>
-  <si>
-    <t>AGOSTO</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>CC</t>
+  </si>
+  <si>
+    <t>NT</t>
   </si>
 </sst>
 </file>
@@ -432,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,405 +471,406 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2">
-        <v>28901342</v>
+        <v>93343273</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F2">
-        <v>1978</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3">
-        <v>20290328</v>
+        <v>1106309469</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D3">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>1963</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>1110545531</v>
+        <v>1109494165</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F4">
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>24486494</v>
+        <v>28890562</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D5">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F5">
-        <v>1976</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6">
-        <v>94516719</v>
+        <v>1110513628</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6">
-        <v>1996</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>93154117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
         <v>15</v>
       </c>
-      <c r="B7">
-        <v>38253096</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7">
-        <v>1980</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8">
-        <v>65769149</v>
+        <v>28898397</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D8">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F8">
-        <v>1994</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>1110574193</v>
+        <v>1005824385</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9">
-        <v>2014</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10">
-        <v>1110549747</v>
+        <v>1109496000</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F10">
-        <v>2010</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>1617567</v>
+        <v>1109496462</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D11">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F11">
-        <v>1956</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>65735017</v>
+        <v>1119583112</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F12">
-        <v>1985</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13">
-        <v>12185483</v>
+        <v>65587237</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13">
-        <v>1972</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>41922408</v>
+        <v>65798919</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D14">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F14">
-        <v>1989</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>28612802</v>
+        <v>28852225</v>
       </c>
       <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="D15">
-        <v>19</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
       <c r="F15">
-        <v>1989</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>28603778</v>
+        <v>1007684243</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D16">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F16">
-        <v>1974</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>65733352</v>
+        <v>65720516</v>
       </c>
       <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
         <v>14</v>
       </c>
-      <c r="D17">
-        <v>22</v>
-      </c>
-      <c r="E17" t="s">
-        <v>10</v>
-      </c>
       <c r="F17">
-        <v>1985</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>28604216</v>
+        <v>65586697</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D18">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F18">
-        <v>1975</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>1109841349</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
         <v>15</v>
       </c>
-      <c r="B19">
-        <v>38257409</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>12</v>
-      </c>
       <c r="F19">
-        <v>1981</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20">
-        <v>65738644</v>
+        <v>36302746</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20">
-        <v>1986</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B21">
-        <v>38261159</v>
+        <v>65588663</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D21">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F21">
-        <v>1982</v>
+        <v>1999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="257" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se arreglo el error del fallo de pagina
</commit_message>
<xml_diff>
--- a/BACKEND/uploads/archivo_subido.xlsx
+++ b/BACKEND/uploads/archivo_subido.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sena\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4966E4C-237C-439E-9900-127208774F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03350240-24A6-43C6-9E60-CEDE37C0A65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>TIPO DE DOCUMENTO</t>
   </si>
@@ -47,27 +47,6 @@
   </si>
   <si>
     <t>NOVIEMBRE</t>
-  </si>
-  <si>
-    <t>JUNIO</t>
-  </si>
-  <si>
-    <t>AGOSTO</t>
-  </si>
-  <si>
-    <t>DICIEMBRE</t>
-  </si>
-  <si>
-    <t>SEPTIEMBRE</t>
-  </si>
-  <si>
-    <t>MAYO</t>
-  </si>
-  <si>
-    <t>OCTUBRE</t>
-  </si>
-  <si>
-    <t>JULIO</t>
   </si>
   <si>
     <t>CC</t>
@@ -436,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,13 +450,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>93343273</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -491,13 +470,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>1106309469</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>19</v>
@@ -511,362 +490,42 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>1109494165</v>
+        <v>65588663</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>2011</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>28890562</v>
+        <v>3042474</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>1971</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>1110513628</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>93154117</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7">
-        <v>1998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>28898397</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8">
-        <v>1972</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>1005824385</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>1109496000</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>1109496462</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <v>1119583112</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>65587237</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13">
-        <v>1991</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>65798919</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14">
-        <v>1994</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>28852225</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15">
-        <v>26</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15">
-        <v>1977</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>1007684243</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>65720516</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17">
-        <v>16</v>
-      </c>
-      <c r="E17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17">
-        <v>1981</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>65586697</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18">
-        <v>28</v>
-      </c>
-      <c r="E18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18">
-        <v>1989</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19">
-        <v>1109841349</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19">
-        <v>14</v>
-      </c>
-      <c r="E19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20">
-        <v>36302746</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20">
-        <v>17</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21">
-        <v>65588663</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21">
-        <v>1999</v>
+        <v>1963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>